<commit_message>
add requested functions and solve general bugs
</commit_message>
<xml_diff>
--- a/arpascm/ARPA_logistics_metrics_v2.0_Scenario_2_al_limite.xlsx
+++ b/arpascm/ARPA_logistics_metrics_v2.0_Scenario_2_al_limite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.pinto\PycharmProjects\ARPA-FCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D39043-67AB-47BA-BFA5-567170C7F6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48714E3C-5D39-4399-AC2E-5314A9C8D214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>file_source</t>
   </si>
@@ -575,16 +575,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.21875" customWidth="1"/>
+    <col min="16" max="16" width="7.77734375" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" customWidth="1"/>
+    <col min="18" max="18" width="9.21875" customWidth="1"/>
+    <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.44140625" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.44140625" customWidth="1"/>
@@ -1594,7 +1600,7 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1606,236 +1612,70 @@
         <v>29</v>
       </c>
       <c r="F13" s="2">
-        <v>44700.14634259259</v>
+        <v>44661.981817129628</v>
       </c>
       <c r="G13" s="2">
-        <v>44702.683136574073</v>
+        <v>44664.322638888887</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13">
-        <v>37.94</v>
+        <v>14.06</v>
       </c>
       <c r="J13">
-        <v>14.93</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="K13">
-        <v>11.02</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="L13">
-        <v>11.99</v>
+        <v>0</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>1044.318454512339</v>
+        <v>1021.389308400584</v>
       </c>
       <c r="O13">
-        <v>60.88</v>
+        <v>56.18</v>
       </c>
       <c r="P13">
-        <v>22.94</v>
+        <v>42.12</v>
       </c>
       <c r="Q13" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="R13" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="S13">
-        <v>39.909999999999997</v>
+        <v>35.130000000000003</v>
       </c>
       <c r="T13">
-        <v>13.96</v>
+        <v>26.08</v>
       </c>
       <c r="U13" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="V13">
-        <v>57.9</v>
+        <v>42.11</v>
       </c>
       <c r="W13">
-        <v>19.96</v>
+        <v>33.06</v>
       </c>
       <c r="X13">
         <v>24.2</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>17.920000000000002</v>
       </c>
       <c r="Z13">
-        <v>0</v>
+        <v>12.86</v>
       </c>
       <c r="AA13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="2">
-        <v>44701.96497685185</v>
-      </c>
-      <c r="G14" s="2">
-        <v>44705.33929398148</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>60.95</v>
-      </c>
-      <c r="J14">
-        <v>51.99</v>
-      </c>
-      <c r="K14">
-        <v>8.9600000000000009</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>1024.376130755493</v>
-      </c>
-      <c r="O14">
-        <v>80.98</v>
-      </c>
-      <c r="P14">
-        <v>20.03</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>48</v>
-      </c>
-      <c r="R14" t="s">
-        <v>49</v>
-      </c>
-      <c r="S14">
-        <v>65</v>
-      </c>
-      <c r="T14">
-        <v>13.01</v>
-      </c>
-      <c r="U14" t="s">
-        <v>50</v>
-      </c>
-      <c r="V14">
-        <v>78.98</v>
-      </c>
-      <c r="W14">
-        <v>18.03</v>
-      </c>
-      <c r="X14">
-        <v>24.2</v>
-      </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15">
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="2">
-        <v>44681.308055555557</v>
-      </c>
-      <c r="G15" s="2">
-        <v>44683.896944444437</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>44.1</v>
-      </c>
-      <c r="J15">
-        <v>1.02</v>
-      </c>
-      <c r="K15">
-        <v>35.07</v>
-      </c>
-      <c r="L15">
-        <v>8.01</v>
-      </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <v>1048.6667262754941</v>
-      </c>
-      <c r="O15">
-        <v>62.13</v>
-      </c>
-      <c r="P15">
-        <v>18.03</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>33</v>
-      </c>
-      <c r="R15" t="s">
-        <v>34</v>
-      </c>
-      <c r="S15">
-        <v>46.11</v>
-      </c>
-      <c r="T15">
-        <v>10.02</v>
-      </c>
-      <c r="U15" t="s">
-        <v>35</v>
-      </c>
-      <c r="V15">
-        <v>61.14</v>
-      </c>
-      <c r="W15">
-        <v>17.04</v>
-      </c>
-      <c r="X15">
-        <v>24.2</v>
-      </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
+        <v>13.41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>